<commit_message>
TICKET4769: added Flex Minimum/Max per Daymora's suggestion
</commit_message>
<xml_diff>
--- a/app/views/packages/xls/PackageNewB.xlsx
+++ b/app/views/packages/xls/PackageNewB.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>%%CLIENT.NAME%%</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Nightly rate based on all-inclusive BAR as found through booking engine</t>
+  </si>
+  <si>
+    <t>Flex Minimum/Max</t>
   </si>
 </sst>
 </file>
@@ -309,32 +312,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -679,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,48 +706,48 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
@@ -766,55 +769,55 @@
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
@@ -822,11 +825,11 @@
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
@@ -834,11 +837,11 @@
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
@@ -863,12 +866,12 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
@@ -886,11 +889,9 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="18"/>
       <c r="E20" s="8"/>
@@ -898,57 +899,69 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>24</v>
+      <c r="A23" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="8"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
TICKET4769: template update to satisfy latest request
</commit_message>
<xml_diff>
--- a/app/views/packages/xls/PackageNewB.xlsx
+++ b/app/views/packages/xls/PackageNewB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>%%CLIENT.NAME%%</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Flex Minimum/Max</t>
+  </si>
+  <si>
+    <t>Number of Rooms</t>
+  </si>
+  <si>
+    <t>%%PACKAGE_NUM_ROOMS%%</t>
   </si>
 </sst>
 </file>
@@ -312,32 +318,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -682,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -706,48 +712,48 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
@@ -769,55 +775,55 @@
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
@@ -825,11 +831,11 @@
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
@@ -837,11 +843,11 @@
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
@@ -866,12 +872,12 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
@@ -889,9 +895,11 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="C20" s="15"/>
       <c r="D20" s="18"/>
       <c r="E20" s="8"/>
@@ -899,11 +907,9 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="18"/>
       <c r="E21" s="8"/>
@@ -911,57 +917,69 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>24</v>
+      <c r="A24" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="8"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>